<commit_message>
overlap.xlsx was not saved, committed now
</commit_message>
<xml_diff>
--- a/p_parameters/archive_parameters/overlap.xlsx
+++ b/p_parameters/archive_parameters/overlap.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>person_id</t>
   </si>
@@ -57,15 +57,9 @@
     <t>matched &lt;- matched[start_match &lt;= i.start_match,]</t>
   </si>
   <si>
-    <t>ORIGIN</t>
-  </si>
-  <si>
     <t>MATCHED</t>
   </si>
   <si>
-    <t>nel dataset ORIGIN etichetti tutti i record id che sono nel dataset MATCHED, con la numerosità delle sue ripetizioni</t>
-  </si>
-  <si>
     <t>quando ordini casualmente metti per ultimi i record con il maggior numero di overlap</t>
   </si>
   <si>
@@ -73,6 +67,15 @@
   </si>
   <si>
     <t>cancelli le ripetizioni, tenendone solo una</t>
+  </si>
+  <si>
+    <t>nel datset MATCHED crei un identificativo di ogni gruppo e ne conti la numerosità</t>
+  </si>
+  <si>
+    <t>nel dataset ORIGIN etichetti tutti i record id che sono nel dataset MATCHED, con la numerosità delle sue ripetizioni e l'identificativo del gruppo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORIGIN: dataset dei </t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,10 +437,10 @@
     <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32" style="1" customWidth="1"/>
+    <col min="12" max="12" width="32" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,29 +462,29 @@
       <c r="J1" t="s">
         <v>2</v>
       </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
       <c r="O1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -503,35 +506,35 @@
       <c r="J2">
         <v>200</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="2">
+      <c r="N2" s="2">
         <v>1</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>3</v>
+      <c r="O2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="2">
+        <v>100</v>
       </c>
       <c r="Q2" s="2">
+        <v>200</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" s="2">
         <v>100</v>
       </c>
-      <c r="R2" s="2">
+      <c r="U2" s="2">
         <v>200</v>
       </c>
-      <c r="S2" s="2">
-        <v>1</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="U2" s="2">
-        <v>100</v>
-      </c>
-      <c r="V2" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -553,32 +556,32 @@
       <c r="J3">
         <v>233</v>
       </c>
-      <c r="O3" s="2">
+      <c r="N3" s="2">
         <v>1</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>3</v>
+      <c r="O3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="2">
+        <v>100</v>
       </c>
       <c r="Q3" s="2">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="R3" s="2">
-        <v>200</v>
-      </c>
-      <c r="S3" s="2">
         <v>2</v>
       </c>
-      <c r="T3" s="2" t="s">
-        <v>3</v>
+      <c r="S3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T3" s="2">
+        <v>125</v>
       </c>
       <c r="U3" s="2">
-        <v>125</v>
-      </c>
-      <c r="V3" s="2">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -600,32 +603,32 @@
       <c r="J4">
         <v>350</v>
       </c>
-      <c r="O4" s="2">
+      <c r="N4" s="2">
         <v>2</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>3</v>
+      <c r="O4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="2">
+        <v>125</v>
       </c>
       <c r="Q4" s="2">
-        <v>125</v>
+        <v>233</v>
       </c>
       <c r="R4" s="2">
-        <v>233</v>
-      </c>
-      <c r="S4" s="2">
         <v>1</v>
       </c>
-      <c r="T4" s="2" t="s">
-        <v>3</v>
+      <c r="S4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T4" s="2">
+        <v>100</v>
       </c>
       <c r="U4" s="2">
-        <v>100</v>
-      </c>
-      <c r="V4" s="2">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -647,176 +650,181 @@
       <c r="J5">
         <v>600</v>
       </c>
-      <c r="O5" s="2">
+      <c r="N5" s="2">
         <v>2</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>3</v>
+      <c r="O5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="2">
+        <v>125</v>
       </c>
       <c r="Q5" s="2">
+        <v>233</v>
+      </c>
+      <c r="R5" s="2">
+        <v>2</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T5" s="2">
         <v>125</v>
       </c>
-      <c r="R5" s="2">
+      <c r="U5" s="2">
         <v>233</v>
       </c>
-      <c r="S5" s="2">
-        <v>2</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="U5" s="2">
-        <v>125</v>
-      </c>
-      <c r="V5" s="2">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O6" s="3">
-        <v>3</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>3</v>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N6" s="3">
+        <v>3</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="3">
+        <v>300</v>
       </c>
       <c r="Q6" s="3">
+        <v>350</v>
+      </c>
+      <c r="R6" s="3">
+        <v>3</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T6" s="3">
         <v>300</v>
       </c>
-      <c r="R6" s="3">
+      <c r="U6" s="3">
         <v>350</v>
       </c>
-      <c r="S6" s="3">
-        <v>3</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U6" s="3">
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="3">
+        <v>3</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="3">
         <v>300</v>
       </c>
-      <c r="V6" s="3">
+      <c r="Q7" s="3">
         <v>350</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="R7" s="3">
+        <v>4</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T7" s="3">
+        <v>325</v>
+      </c>
+      <c r="U7" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N8" s="3">
+        <v>4</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="3">
+        <v>325</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>600</v>
+      </c>
+      <c r="R8" s="3">
+        <v>3</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T8" s="3">
+        <v>300</v>
+      </c>
+      <c r="U8" s="3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N9" s="3">
+        <v>4</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="3">
+        <v>325</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>600</v>
+      </c>
+      <c r="R9" s="3">
+        <v>4</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T9" s="3">
+        <v>325</v>
+      </c>
+      <c r="U9" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="N11" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="3">
-        <v>3</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>300</v>
-      </c>
-      <c r="R7" s="3">
-        <v>350</v>
-      </c>
-      <c r="S7" s="3">
-        <v>4</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U7" s="3">
-        <v>325</v>
-      </c>
-      <c r="V7" s="3">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O8" s="3">
-        <v>4</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>325</v>
-      </c>
-      <c r="R8" s="3">
-        <v>600</v>
-      </c>
-      <c r="S8" s="3">
-        <v>3</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U8" s="3">
-        <v>300</v>
-      </c>
-      <c r="V8" s="3">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O9" s="3">
-        <v>4</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>325</v>
-      </c>
-      <c r="R9" s="3">
-        <v>600</v>
-      </c>
-      <c r="S9" s="3">
-        <v>4</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U9" s="3">
-        <v>325</v>
-      </c>
-      <c r="V9" s="3">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>